<commit_message>
sync，add hybridclr, fix some problems
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/StartConfig/Benchmark/StartSceneConfig@s.xlsx
+++ b/Unity/Assets/Config/Excel/StartConfig/Benchmark/StartSceneConfig@s.xlsx
@@ -159,10 +159,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -184,6 +184,65 @@
       <color theme="1"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -196,25 +255,54 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -226,44 +314,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -276,59 +329,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -345,6 +345,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -357,6 +405,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -369,49 +447,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,109 +525,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,11 +541,59 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -568,23 +616,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,49 +636,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -654,133 +654,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1150,7 +1150,7 @@
   <dimension ref="B3:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1241,7 +1241,7 @@
         <v>13</v>
       </c>
       <c r="H6" s="5">
-        <v>10002</v>
+        <v>30001</v>
       </c>
     </row>
     <row r="7" spans="3:8">
@@ -1261,7 +1261,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="5">
-        <v>10003</v>
+        <v>30002</v>
       </c>
     </row>
     <row r="8" spans="3:8">
@@ -1281,7 +1281,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="5">
-        <v>10004</v>
+        <v>30003</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -1304,7 +1304,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="5">
-        <v>10005</v>
+        <v>30004</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -1327,7 +1327,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>10006</v>
+        <v>30005</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -1350,7 +1350,7 @@
         <v>20</v>
       </c>
       <c r="H11" s="5">
-        <v>10007</v>
+        <v>30006</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="2:8">
@@ -1373,7 +1373,7 @@
         <v>21</v>
       </c>
       <c r="H12" s="5">
-        <v>10008</v>
+        <v>30007</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" spans="2:8">
@@ -1396,7 +1396,7 @@
         <v>22</v>
       </c>
       <c r="H13" s="5">
-        <v>10009</v>
+        <v>30008</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="2:8">
@@ -1419,7 +1419,7 @@
         <v>23</v>
       </c>
       <c r="H14" s="5">
-        <v>10010</v>
+        <v>30009</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" spans="2:8">
@@ -1442,7 +1442,7 @@
         <v>24</v>
       </c>
       <c r="H15" s="5">
-        <v>10011</v>
+        <v>30010</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" spans="2:8">
@@ -1465,7 +1465,7 @@
         <v>25</v>
       </c>
       <c r="H16" s="5">
-        <v>10012</v>
+        <v>30011</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" spans="2:8">
@@ -1488,7 +1488,7 @@
         <v>26</v>
       </c>
       <c r="H17" s="5">
-        <v>10013</v>
+        <v>30012</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" spans="2:8">
@@ -1511,7 +1511,7 @@
         <v>27</v>
       </c>
       <c r="H18" s="5">
-        <v>10014</v>
+        <v>30013</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" spans="2:8">
@@ -1534,7 +1534,7 @@
         <v>28</v>
       </c>
       <c r="H19" s="5">
-        <v>10015</v>
+        <v>30014</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" spans="2:8">
@@ -1557,7 +1557,7 @@
         <v>29</v>
       </c>
       <c r="H20" s="5">
-        <v>10016</v>
+        <v>30015</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="2:8">
@@ -1580,7 +1580,7 @@
         <v>30</v>
       </c>
       <c r="H21" s="5">
-        <v>10017</v>
+        <v>30016</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" spans="2:8">
@@ -1603,7 +1603,7 @@
         <v>31</v>
       </c>
       <c r="H22" s="5">
-        <v>10018</v>
+        <v>30017</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" spans="2:8">
@@ -1626,7 +1626,7 @@
         <v>32</v>
       </c>
       <c r="H23" s="5">
-        <v>10019</v>
+        <v>30018</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" spans="2:8">
@@ -1649,7 +1649,7 @@
         <v>33</v>
       </c>
       <c r="H24" s="5">
-        <v>10020</v>
+        <v>30019</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" spans="2:8">
@@ -1672,7 +1672,7 @@
         <v>34</v>
       </c>
       <c r="H25" s="5">
-        <v>10021</v>
+        <v>30020</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" spans="2:8">
@@ -1695,7 +1695,7 @@
         <v>35</v>
       </c>
       <c r="H26" s="5">
-        <v>10022</v>
+        <v>30021</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" spans="2:8">
@@ -1718,7 +1718,7 @@
         <v>36</v>
       </c>
       <c r="H27" s="5">
-        <v>10023</v>
+        <v>30022</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" spans="2:8">
@@ -1741,7 +1741,7 @@
         <v>37</v>
       </c>
       <c r="H28" s="5">
-        <v>10024</v>
+        <v>30023</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" spans="2:8">
@@ -1764,7 +1764,7 @@
         <v>38</v>
       </c>
       <c r="H29" s="5">
-        <v>10025</v>
+        <v>30024</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" spans="2:8">
@@ -1787,7 +1787,7 @@
         <v>39</v>
       </c>
       <c r="H30" s="5">
-        <v>10026</v>
+        <v>30025</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" spans="2:8">
@@ -1810,7 +1810,7 @@
         <v>40</v>
       </c>
       <c r="H31" s="5">
-        <v>10027</v>
+        <v>30026</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" spans="2:8">
@@ -1833,7 +1833,7 @@
         <v>41</v>
       </c>
       <c r="H32" s="5">
-        <v>10028</v>
+        <v>30027</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" spans="2:8">
@@ -1856,7 +1856,7 @@
         <v>42</v>
       </c>
       <c r="H33" s="5">
-        <v>10029</v>
+        <v>30028</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" spans="2:8">
@@ -1879,7 +1879,7 @@
         <v>43</v>
       </c>
       <c r="H34" s="5">
-        <v>10030</v>
+        <v>30029</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" spans="2:8">
@@ -1902,7 +1902,7 @@
         <v>44</v>
       </c>
       <c r="H35" s="5">
-        <v>10031</v>
+        <v>30030</v>
       </c>
     </row>
     <row r="36" s="2" customFormat="1" spans="2:8">
@@ -1925,7 +1925,7 @@
         <v>45</v>
       </c>
       <c r="H36" s="5">
-        <v>10032</v>
+        <v>30031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>